<commit_message>
Update Codebooks w.r.t. levels and amount of needs
</commit_message>
<xml_diff>
--- a/annotation/annotation_schema_cookversational_search.xlsx
+++ b/annotation/annotation_schema_cookversational_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\Documents\Arbeit\Konferenzen\TOIS\CookversationalSearch\annotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\Google Drive\Promotion\CookversationalSearch\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B706DFB-F49B-4502-B233-F417D14514DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AD0480-1F9F-461B-AE5E-A01D4406748E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17196" yWindow="6336" windowWidth="23040" windowHeight="12204" firstSheet="8" activeTab="12" xr2:uid="{4DA8BC8C-CB17-4341-84BF-B96DC8599B67}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{4DA8BC8C-CB17-4341-84BF-B96DC8599B67}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="3" r:id="rId1"/>
@@ -24,8 +24,7 @@
     <sheet name="Knowledge" sheetId="10" r:id="rId9"/>
     <sheet name="Meal" sheetId="11" r:id="rId10"/>
     <sheet name="Temperature" sheetId="12" r:id="rId11"/>
-    <sheet name="Actions &amp; Commands" sheetId="13" r:id="rId12"/>
-    <sheet name="Misc" sheetId="14" r:id="rId13"/>
+    <sheet name="Misc" sheetId="14" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">Overview!#REF!</definedName>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="592">
   <si>
     <t>Definition</t>
   </si>
@@ -221,39 +220,9 @@
     <t>Cooking Time</t>
   </si>
   <si>
-    <t>Do Calculations</t>
-  </si>
-  <si>
-    <t>Pause reading out</t>
-  </si>
-  <si>
-    <t>Turn on music</t>
-  </si>
-  <si>
     <t>Ingredient Substitution</t>
   </si>
   <si>
-    <t>Add Ingredients to Recipe Search</t>
-  </si>
-  <si>
-    <t>Change Amount of Ingredient</t>
-  </si>
-  <si>
-    <t>Change Amount of Persons</t>
-  </si>
-  <si>
-    <t>Recipe Adaption</t>
-  </si>
-  <si>
-    <t>Filter Search</t>
-  </si>
-  <si>
-    <t>Navigation - Recipe Ingredient List</t>
-  </si>
-  <si>
-    <t>Navigation - Switch back to recipe</t>
-  </si>
-  <si>
     <t>Read out result list</t>
   </si>
   <si>
@@ -614,12 +583,6 @@
     <t>Request for Recipe Search Success</t>
   </si>
   <si>
-    <t>Recipe selection - explizit</t>
-  </si>
-  <si>
-    <t>Recipe selection - implicit</t>
-  </si>
-  <si>
     <t>Miscellaneous</t>
   </si>
   <si>
@@ -656,30 +619,9 @@
     <t>Experience</t>
   </si>
   <si>
-    <t>„Pause (,)“ (TP36, Absatz 55)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingredient removal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repeat Ingredient Readout </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recipe Selection </t>
-  </si>
-  <si>
-    <t>Change Amount</t>
-  </si>
-  <si>
-    <t>Codes</t>
-  </si>
-  <si>
     <t>Cooking Technique</t>
   </si>
   <si>
-    <t>Actions &amp; Commands</t>
-  </si>
-  <si>
     <t xml:space="preserve">Next Ingredient </t>
   </si>
   <si>
@@ -689,15 +631,6 @@
     <t>Temperature Reassurance</t>
   </si>
   <si>
-    <t>Timer</t>
-  </si>
-  <si>
-    <t>Bookmark</t>
-  </si>
-  <si>
-    <t>Navigational Instruction on SERP</t>
-  </si>
-  <si>
     <t>Question regarding experiment</t>
   </si>
   <si>
@@ -734,9 +667,6 @@
     <t>Information needs relating to temperature.</t>
   </si>
   <si>
-    <t>Utterances of this class cannot be viewed as formal information needs. They include commands and actions users can pose to the system.</t>
-  </si>
-  <si>
     <t>Information needs that cannot be assigned to one of the aforementioned classes.</t>
   </si>
   <si>
@@ -1325,78 +1255,6 @@
     <t>Question regarding the temperature</t>
   </si>
   <si>
-    <t>Command to substitute an ingredient</t>
-  </si>
-  <si>
-    <t>Command to the system to do calculations</t>
-  </si>
-  <si>
-    <t>Command to pause reading out steps/ingredients etc.</t>
-  </si>
-  <si>
-    <t>Command to set/modify/stop the timer</t>
-  </si>
-  <si>
-    <t>Command to turn on music</t>
-  </si>
-  <si>
-    <t>Command to remove/leave out ingredients</t>
-  </si>
-  <si>
-    <t>Command to repeat an ingredient</t>
-  </si>
-  <si>
-    <t>Message for the system to select a recipe</t>
-  </si>
-  <si>
-    <t>Explicit selection of a recipe</t>
-  </si>
-  <si>
-    <t>Implicit selection of a recipe</t>
-  </si>
-  <si>
-    <t>Command to change amounts</t>
-  </si>
-  <si>
-    <t>Command to change the amount of an ingredient</t>
-  </si>
-  <si>
-    <t>Command to change the number of persons for which the recipe is meant</t>
-  </si>
-  <si>
-    <t>Adaptation of the recipe. Entire parts of the preparation are substituted.</t>
-  </si>
-  <si>
-    <t>User Command</t>
-  </si>
-  <si>
-    <t>User Search Actions</t>
-  </si>
-  <si>
-    <t>Add a specific filter to the recipe search</t>
-  </si>
-  <si>
-    <t>System should navigate in the ingredient list of a recipe</t>
-  </si>
-  <si>
-    <t>User wants to mark the recipe down</t>
-  </si>
-  <si>
-    <t>Desire to talk about the recipe again/ to switch back to the recipe. This constitutes an act of navigation.</t>
-  </si>
-  <si>
-    <t>System Instruction - Stop Reading out SERP</t>
-  </si>
-  <si>
-    <t>The system should stop reading out the SERP</t>
-  </si>
-  <si>
-    <t>Navigational instructions on the SERP. The user has a mental model of the website.</t>
-  </si>
-  <si>
-    <t>Command to add ingredients to the recipe search</t>
-  </si>
-  <si>
     <t>Question if the utensil needs to be changed during the preparation. The reason for that is the planning of the procedure.</t>
   </si>
   <si>
@@ -1430,9 +1288,6 @@
     <t xml:space="preserve">User wants to know the "system's" (experimenter's ) experience </t>
   </si>
   <si>
-    <t>Code Level 1</t>
-  </si>
-  <si>
     <t>Code Level 2</t>
   </si>
   <si>
@@ -1440,9 +1295,6 @@
   </si>
   <si>
     <t>Code Level 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code Level 2 </t>
   </si>
   <si>
     <t>„Ok (_) Dann (-) Geh ich jetzt einfach mal davon aus dass (-) eine halbe Zwiebel ungefähr zwei Schalotten entspricht (?)“ (TP14, Absatz 120) -- "Ok. I suppose half an onion is the same as two shallots?" (part. 14, paragraph 120)</t>
@@ -1941,60 +1793,6 @@
     <t xml:space="preserve">„Bei wie viel Temperatur (?)“ (TP13, Absatz 40) -- "At how much temperature (?)" (part. 13, paragraph 40) </t>
   </si>
   <si>
-    <t>„Wir ersetzen Frischkäse durch Mozzarella (_)“ (TP30, Absatz 173) -- "We replace cream cheese with mozzarella (_)" (part. 30, paragraph 173)</t>
-  </si>
-  <si>
-    <t>„Kannst du mir das ausrechnen (?)“ (TP39, Absatz 21) -- "Can you calculate this for me (?)" (part. 39, paragraph 21)</t>
-  </si>
-  <si>
-    <t>„Gut (-) Wecker auf 45 Minuten (_)“ (TP35, Absatz 97) -- "Good (-) alarm clock is set at 45 minutes (_)" (part. 35, paragraph 97)</t>
-  </si>
-  <si>
-    <t>„Alex (_) Schalte Musik ein (_)“ (TP30, Absatz 61) -- "Alex (_) turn on the music (_)" (part. 30, paragraph 61)</t>
-  </si>
-  <si>
-    <t>„Schinken kannst weglassen (_)“ (TP1, Absatz 164) -- "You can leave out the ham (_)" (part. 1, paragraph 164)</t>
-  </si>
-  <si>
-    <t>„Was war da nochmal les nochmal vor (-)“ (TP21, Absatz 18) -- "What was there (?) Read it out to me (-)" (part. 21, paragraph 18)</t>
-  </si>
-  <si>
-    <t>„Ja das hört sich doch gut an (_) Dann machen wir das (,)“ (TP13, Absatz 10) -- "Yes, that sounds good (_) Then we do it (,)" (part. 13, paragraph 10)</t>
-  </si>
-  <si>
-    <t>„Perfekt (,) Klingt gut (_)“ (TP7, Absatz 26) -- "Perfect (,) Sounds good (_)" (part. 7, paragraph 26)</t>
-  </si>
-  <si>
-    <t>„Reduziere die Menge auf die Hälfte“ (TP30, Absatz 53) -- "Reduce the amount by half" (part. 30, paragraph 53)</t>
-  </si>
-  <si>
-    <t>„Für zwei Personen (_)“ (TP39, Absatz 19) -- "For two people (_)" (part. 39, paragraph 19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">„Nö wir machen es vegetarisch (_)“ (TP6, Absatz 16) -- "Nope we'll make it vegetarian (_)" (part. 6, paragraph 16) </t>
-  </si>
-  <si>
-    <t>„Und nimm alles raus was überbacken werden muss oder einen Ofen braucht (_)“ (TP25, Absatz 4) -- "And leave out everything that needs to be baked or needs an oven (_)" (part. 25, paragraph 4)</t>
-  </si>
-  <si>
-    <t>„Oder steht vielleicht bei den ZUtaten schau nochmal da (,) bei den Zutaten steht ja dann auch manchmal (-)“ (TP23, Absatz 44) -- "Or maybe we find it in the ingredients list (,) have a look (-)" (part. 23, paragraph 44)</t>
-  </si>
-  <si>
-    <t>„Kannst du da irgendwie vormerken oder so (?)“ (TP21, Absatz 12) -- "Can you make a note or something (?)" (part. 21, paragraph 12)</t>
-  </si>
-  <si>
-    <t>„Ok dann tu mal wieder das Rezept her (,)(.)“ (TP1, Absatz 102) -- "Ok then show me the recipe again (,) (.)" (part. 1, paragraph 102)</t>
-  </si>
-  <si>
-    <t>„//Ja passt schon//(_)“ (TP1, Absatz 212) -- "// Yes that's fine // (_)" (part. 1, paragraph 212)</t>
-  </si>
-  <si>
-    <t>„Geh mal ganz oben in das ähm (..) da wo die an Sterne angezeigt werden (_)“ (TP1, Absatz 42) -- "Go to the top of the um (..) where the stars are displayed (_)" (part. 1, paragraph 42)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">„Vielleicht kannst du noch irgendwie Zutaten dazu (?) geben (,)“ (TP14, Absatz 10) -- "Maybe you can somehow add ingredients (?)" (part. 14, paragraph 10) </t>
-  </si>
-  <si>
     <t>„Wechsel ich das Gefäß noch einmal (_)“ (TP30, Absatz 91) -- "Do I change the vessel again (_)" (part. 30, paragraph 91)</t>
   </si>
   <si>
@@ -2026,6 +1824,12 @@
   </si>
   <si>
     <t xml:space="preserve">„Hast du schon mal die (-) Reis so gekocht (?)“ (TP8, Absatz 164) -- "Have you ever cooked (-) rice like this (?)" (part. 8, paragraph 164) </t>
+  </si>
+  <si>
+    <t>Codes Level 1</t>
+  </si>
+  <si>
+    <t>Code Level 5</t>
   </si>
 </sst>
 </file>
@@ -2206,7 +2010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2256,9 +2060,6 @@
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2291,9 +2092,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2335,10 +2133,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B42E45A7-EF15-44AA-A868-BBE9DA6AFCB1}" name="Tabelle1" displayName="Tabelle1" ref="A1:B13" totalsRowShown="0">
-  <autoFilter ref="A1:B13" xr:uid="{43E75D6E-17FA-4284-B00D-13ADAD35587D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B42E45A7-EF15-44AA-A868-BBE9DA6AFCB1}" name="Tabelle1" displayName="Tabelle1" ref="A1:B12" totalsRowShown="0">
+  <autoFilter ref="A1:B12" xr:uid="{43E75D6E-17FA-4284-B00D-13ADAD35587D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0B559FDF-4413-4370-B9ED-7B8E27C4885E}" name="Codes"/>
+    <tableColumn id="1" xr3:uid="{0B559FDF-4413-4370-B9ED-7B8E27C4885E}" name="Codes Level 1"/>
     <tableColumn id="2" xr3:uid="{399351BD-80B6-4288-B4BE-4CA149F055A3}" name="Definition" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2642,10 +2440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B401E1D3-9445-4B4C-A072-A2434CC2F18B}">
-  <dimension ref="A1:F238"/>
+  <dimension ref="A1:F237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2662,7 +2460,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>205</v>
+        <v>590</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2672,50 +2470,50 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
@@ -2725,7 +2523,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="E7"/>
       <c r="F7"/>
@@ -2735,7 +2533,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="E8"/>
       <c r="F8"/>
@@ -2745,7 +2543,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="E9"/>
       <c r="F9"/>
@@ -2755,39 +2553,33 @@
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>226</v>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="E13"/>
       <c r="F13"/>
     </row>
@@ -3686,10 +3478,6 @@
     <row r="237" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E237"/>
       <c r="F237"/>
-    </row>
-    <row r="238" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E238"/>
-      <c r="F238"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3704,8 +3492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C654C72-2A14-48F0-AC22-9EDF2E09CA5B}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3716,26 +3504,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -3748,10 +3536,10 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>408</v>
+        <v>385</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>613</v>
+        <v>564</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -3764,10 +3552,10 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>614</v>
+        <v>565</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -3780,10 +3568,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>615</v>
+        <v>566</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -3796,10 +3584,10 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>616</v>
+        <v>567</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -3814,10 +3602,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>412</v>
+        <v>389</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>617</v>
+        <v>568</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -3830,10 +3618,10 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>618</v>
+        <v>569</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -3846,10 +3634,10 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>619</v>
+        <v>570</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -3862,10 +3650,10 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>415</v>
+        <v>392</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>620</v>
+        <v>571</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -3881,8 +3669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D71A272-7C83-4B66-A33D-2AE2C4E95D09}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3893,26 +3681,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="21" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -3921,14 +3709,14 @@
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>621</v>
+        <v>572</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -3937,14 +3725,14 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>417</v>
+        <v>394</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>622</v>
+        <v>573</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -3953,14 +3741,14 @@
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>418</v>
+        <v>395</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>623</v>
+        <v>574</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -3969,21 +3757,21 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>625</v>
+        <v>576</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="4" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -3995,13 +3783,13 @@
         <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>420</v>
+        <v>397</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>624</v>
+        <v>575</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -4010,13 +3798,13 @@
         <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>421</v>
+        <v>398</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>626</v>
+        <v>577</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -4025,14 +3813,14 @@
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>627</v>
+        <v>578</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -4045,404 +3833,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F915427E-EB66-4D57-9EE6-CCE54387639F}">
-  <dimension ref="A1:F27"/>
-  <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="53.5546875" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" customWidth="1"/>
-    <col min="4" max="4" width="76.109375" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="36" t="s">
-        <v>437</v>
-      </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>628</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>629</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>630</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>637</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="16"/>
-      <c r="C26" s="23"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="16"/>
-      <c r="C27" s="23"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B0DF86-2410-4906-BE52-F9521CE6C0DA}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4454,26 +3849,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -4482,14 +3877,14 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>447</v>
+        <v>400</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>646</v>
+        <v>579</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -4498,14 +3893,14 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>448</v>
+        <v>401</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>647</v>
+        <v>580</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -4514,14 +3909,14 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>449</v>
+        <v>402</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>648</v>
+        <v>581</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -4530,14 +3925,14 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>450</v>
+        <v>403</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>649</v>
+        <v>582</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -4546,14 +3941,14 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>451</v>
+        <v>404</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>650</v>
+        <v>583</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -4565,13 +3960,13 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>452</v>
+        <v>405</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>651</v>
+        <v>584</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -4580,14 +3975,14 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>453</v>
+        <v>406</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>652</v>
+        <v>585</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -4596,14 +3991,14 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
-        <v>454</v>
+        <v>407</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>653</v>
+        <v>586</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -4612,14 +4007,14 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>455</v>
+        <v>408</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>654</v>
+        <v>587</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -4628,14 +4023,14 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>456</v>
+        <v>409</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>655</v>
+        <v>588</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -4644,14 +4039,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
-        <v>457</v>
+        <v>410</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>656</v>
+        <v>589</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -4667,8 +4062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97EE1575-6DD2-47BE-8FAF-B6DF066CFA3D}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4681,26 +4076,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -4709,14 +4104,14 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>463</v>
+        <v>414</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -4725,14 +4120,14 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>465</v>
+        <v>416</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -4741,14 +4136,14 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>464</v>
+        <v>415</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -4757,14 +4152,14 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>466</v>
+        <v>417</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -4773,11 +4168,11 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2"/>
@@ -4793,10 +4188,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>467</v>
+        <v>418</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -4808,13 +4203,13 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>468</v>
+        <v>419</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -4826,13 +4221,13 @@
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>469</v>
+        <v>420</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -4844,13 +4239,13 @@
         <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>470</v>
+        <v>421</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -4859,14 +4254,14 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>471</v>
+        <v>422</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -4875,14 +4270,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>472</v>
+        <v>423</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -4891,13 +4286,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>473</v>
+        <v>424</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -4906,13 +4301,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>474</v>
+        <v>425</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -4921,14 +4316,14 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>475</v>
+        <v>426</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -4937,13 +4332,13 @@
         <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>476</v>
+        <v>427</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -4952,13 +4347,13 @@
         <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>477</v>
+        <v>428</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -4974,8 +4369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE098B1-1A9F-4D55-8585-A671B6D9B9D3}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="E45" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4991,31 +4386,31 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
-      <c r="B1" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="7" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>460</v>
+        <v>413</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -5024,12 +4419,12 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -5042,11 +4437,11 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -5062,13 +4457,13 @@
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>481</v>
+        <v>432</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -5083,13 +4478,13 @@
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>480</v>
+        <v>431</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -5101,14 +4496,14 @@
         <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>479</v>
+        <v>430</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -5120,14 +4515,14 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>478</v>
+        <v>429</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -5139,14 +4534,14 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>482</v>
+        <v>433</v>
       </c>
       <c r="G9" s="3"/>
     </row>
@@ -5158,11 +4553,11 @@
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -5178,13 +4573,13 @@
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>483</v>
+        <v>434</v>
       </c>
       <c r="G11" s="3"/>
     </row>
@@ -5199,13 +4594,13 @@
         <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>484</v>
+        <v>435</v>
       </c>
       <c r="G12" s="3"/>
     </row>
@@ -5221,10 +4616,10 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>485</v>
+        <v>436</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -5236,14 +4631,14 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>486</v>
+        <v>437</v>
       </c>
       <c r="G14" s="3"/>
     </row>
@@ -5252,15 +4647,15 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>487</v>
+        <v>438</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -5269,15 +4664,15 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>488</v>
+        <v>439</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -5289,14 +4684,14 @@
         <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>489</v>
+        <v>440</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -5308,14 +4703,14 @@
         <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>490</v>
+        <v>441</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -5324,15 +4719,15 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>491</v>
+        <v>442</v>
       </c>
       <c r="G19" s="3"/>
     </row>
@@ -5341,12 +4736,12 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -5359,14 +4754,14 @@
         <v>12</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>492</v>
+        <v>443</v>
       </c>
       <c r="G21" s="3"/>
     </row>
@@ -5378,14 +4773,14 @@
         <v>12</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>493</v>
+        <v>444</v>
       </c>
       <c r="G22" s="3"/>
     </row>
@@ -5401,10 +4796,10 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>494</v>
+        <v>445</v>
       </c>
       <c r="G23" s="3"/>
     </row>
@@ -5416,14 +4811,14 @@
         <v>12</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>495</v>
+        <v>446</v>
       </c>
       <c r="G24" s="3"/>
     </row>
@@ -5435,14 +4830,14 @@
         <v>12</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>496</v>
+        <v>447</v>
       </c>
       <c r="G25" s="3"/>
     </row>
@@ -5454,14 +4849,14 @@
         <v>12</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>497</v>
+        <v>448</v>
       </c>
       <c r="G26" s="3"/>
     </row>
@@ -5470,15 +4865,15 @@
         <v>12</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>498</v>
+        <v>449</v>
       </c>
       <c r="G27" s="3"/>
     </row>
@@ -5487,12 +4882,12 @@
         <v>12</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -5505,14 +4900,14 @@
         <v>12</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>499</v>
+        <v>450</v>
       </c>
       <c r="G29" s="3"/>
     </row>
@@ -5524,14 +4919,14 @@
         <v>12</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>500</v>
+        <v>451</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -5543,14 +4938,14 @@
         <v>12</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>499</v>
+        <v>450</v>
       </c>
       <c r="G31" s="3"/>
     </row>
@@ -5566,10 +4961,10 @@
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>501</v>
+        <v>452</v>
       </c>
       <c r="G32" s="3"/>
     </row>
@@ -5578,12 +4973,12 @@
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -5600,10 +4995,10 @@
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>502</v>
+        <v>453</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -5615,14 +5010,14 @@
         <v>12</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>503</v>
+        <v>454</v>
       </c>
       <c r="G35" s="3"/>
     </row>
@@ -5634,14 +5029,14 @@
         <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>504</v>
+        <v>455</v>
       </c>
       <c r="G36" s="3"/>
     </row>
@@ -5653,14 +5048,14 @@
         <v>12</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>505</v>
+        <v>456</v>
       </c>
       <c r="G37" s="3"/>
     </row>
@@ -5669,12 +5064,12 @@
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -5691,10 +5086,10 @@
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>507</v>
+        <v>458</v>
       </c>
       <c r="G39" s="3"/>
     </row>
@@ -5706,14 +5101,14 @@
         <v>12</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>506</v>
+        <v>457</v>
       </c>
       <c r="G40" s="3"/>
     </row>
@@ -5725,14 +5120,14 @@
         <v>12</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>508</v>
+        <v>459</v>
       </c>
       <c r="G41" s="3"/>
     </row>
@@ -5744,14 +5139,14 @@
         <v>12</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>509</v>
+        <v>460</v>
       </c>
       <c r="G42" s="3"/>
     </row>
@@ -5760,15 +5155,15 @@
         <v>12</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>510</v>
+        <v>461</v>
       </c>
       <c r="G43" s="3"/>
     </row>
@@ -5777,12 +5172,12 @@
         <v>12</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -5795,14 +5190,14 @@
         <v>12</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>511</v>
+        <v>462</v>
       </c>
       <c r="G45" s="3"/>
     </row>
@@ -5818,10 +5213,10 @@
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>512</v>
+        <v>463</v>
       </c>
       <c r="G46" s="3"/>
     </row>
@@ -5833,14 +5228,14 @@
         <v>12</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>513</v>
+        <v>464</v>
       </c>
       <c r="G47" s="3"/>
     </row>
@@ -5852,14 +5247,14 @@
         <v>12</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>514</v>
+        <v>465</v>
       </c>
       <c r="G48" s="3"/>
     </row>
@@ -5868,12 +5263,12 @@
         <v>12</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -5886,14 +5281,14 @@
         <v>12</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="G50" s="3"/>
     </row>
@@ -5905,7 +5300,7 @@
         <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -5923,13 +5318,13 @@
         <v>12</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="G52" s="3"/>
     </row>
@@ -5944,13 +5339,13 @@
         <v>12</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>517</v>
+        <v>468</v>
       </c>
       <c r="G53" s="3"/>
     </row>
@@ -5965,13 +5360,13 @@
         <v>12</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
       <c r="G54" s="3"/>
     </row>
@@ -5983,7 +5378,7 @@
         <v>12</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -6001,13 +5396,13 @@
         <v>12</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
       <c r="G56" s="3"/>
     </row>
@@ -6022,13 +5417,13 @@
         <v>12</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
       <c r="G57" s="3"/>
     </row>
@@ -6043,13 +5438,13 @@
         <v>12</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
       <c r="G58" s="3"/>
     </row>
@@ -6064,13 +5459,13 @@
         <v>12</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
       <c r="G59" s="3"/>
     </row>
@@ -6082,14 +5477,14 @@
         <v>12</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>523</v>
+        <v>474</v>
       </c>
       <c r="G60" s="3"/>
     </row>
@@ -6105,10 +5500,10 @@
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>524</v>
+        <v>475</v>
       </c>
       <c r="G61" s="3"/>
     </row>
@@ -6124,8 +5519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07392A47-5175-4595-BC44-1650A45F3926}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6138,26 +5533,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>462</v>
+        <v>412</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -6166,11 +5561,11 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -6183,13 +5578,13 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>525</v>
+        <v>476</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -6201,13 +5596,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>526</v>
+        <v>477</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -6219,13 +5614,13 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>527</v>
+        <v>478</v>
       </c>
       <c r="F6" s="3"/>
     </row>
@@ -6237,13 +5632,13 @@
         <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>528</v>
+        <v>479</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -6255,13 +5650,13 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>529</v>
+        <v>480</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -6273,13 +5668,13 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>530</v>
+        <v>481</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -6291,13 +5686,13 @@
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>531</v>
+        <v>482</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -6309,13 +5704,13 @@
         <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>532</v>
+        <v>483</v>
       </c>
       <c r="F11" s="3"/>
     </row>
@@ -6327,13 +5722,13 @@
         <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>533</v>
+        <v>484</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -6345,13 +5740,13 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>534</v>
+        <v>485</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -6363,13 +5758,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>535</v>
+        <v>486</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -6381,13 +5776,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>536</v>
+        <v>487</v>
       </c>
       <c r="F15" s="3"/>
     </row>
@@ -6399,13 +5794,13 @@
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>537</v>
+        <v>488</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -6414,14 +5809,14 @@
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>538</v>
+        <v>489</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -6430,14 +5825,14 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>539</v>
+        <v>490</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -6446,14 +5841,14 @@
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>540</v>
+        <v>491</v>
       </c>
       <c r="F19" s="3"/>
     </row>
@@ -6462,14 +5857,14 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>541</v>
+        <v>492</v>
       </c>
       <c r="F20" s="3"/>
     </row>
@@ -6478,14 +5873,14 @@
         <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>324</v>
+        <v>301</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>542</v>
+        <v>493</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -6501,8 +5896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A411C0C-28B1-4379-A4D6-C3F45C1C4DE2}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6514,26 +5909,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -6542,14 +5937,14 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>325</v>
+        <v>302</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>543</v>
+        <v>494</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -6558,14 +5953,14 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>544</v>
+        <v>495</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -6574,14 +5969,14 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>545</v>
+        <v>496</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -6590,14 +5985,14 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>546</v>
+        <v>497</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -6606,14 +6001,14 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>547</v>
+        <v>498</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -6622,11 +6017,11 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>330</v>
+        <v>307</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
@@ -6639,13 +6034,13 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>331</v>
+        <v>308</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>548</v>
+        <v>499</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -6657,13 +6052,13 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>332</v>
+        <v>309</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>549</v>
+        <v>500</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -6672,14 +6067,14 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>550</v>
+        <v>501</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -6688,14 +6083,14 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>551</v>
+        <v>502</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -6704,14 +6099,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>552</v>
+        <v>503</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -6727,8 +6122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37B65F74-2026-4F89-81A2-27E36103C220}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6740,27 +6135,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="15" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -6773,7 +6168,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
@@ -6789,10 +6184,10 @@
         <v>36</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>553</v>
+        <v>504</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -6807,10 +6202,10 @@
         <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>554</v>
+        <v>505</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -6823,7 +6218,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
@@ -6839,10 +6234,10 @@
         <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>555</v>
+        <v>506</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -6857,10 +6252,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>341</v>
+        <v>318</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>556</v>
+        <v>507</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -6873,10 +6268,10 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>557</v>
+        <v>508</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -6889,7 +6284,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
@@ -6905,10 +6300,10 @@
         <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>558</v>
+        <v>509</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -6923,10 +6318,10 @@
         <v>44</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>345</v>
+        <v>322</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>559</v>
+        <v>510</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -6939,10 +6334,10 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>346</v>
+        <v>323</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>560</v>
+        <v>511</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -6955,10 +6350,10 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>347</v>
+        <v>324</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>561</v>
+        <v>512</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -6971,10 +6366,10 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>348</v>
+        <v>325</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>562</v>
+        <v>513</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -6987,7 +6382,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>349</v>
+        <v>326</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
@@ -7003,10 +6398,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>350</v>
+        <v>327</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>563</v>
+        <v>514</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -7021,10 +6416,10 @@
         <v>49</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>351</v>
+        <v>328</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>564</v>
+        <v>515</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -7039,10 +6434,10 @@
         <v>50</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>565</v>
+        <v>516</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -7055,7 +6450,7 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>353</v>
+        <v>330</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
@@ -7071,10 +6466,10 @@
         <v>18</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>566</v>
+        <v>517</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -7089,10 +6484,10 @@
         <v>52</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>355</v>
+        <v>332</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>567</v>
+        <v>518</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -7107,10 +6502,10 @@
         <v>53</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>356</v>
+        <v>333</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>568</v>
+        <v>519</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -7123,10 +6518,10 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>569</v>
+        <v>520</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -7142,8 +6537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EFF3A2-12C7-4554-942E-AC5C50C03C75}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="F15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7157,35 +6552,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="B1" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="13" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>460</v>
+        <v>413</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>461</v>
+        <v>591</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="H2" s="14"/>
     </row>
@@ -7194,16 +6589,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>570</v>
+        <v>521</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -7212,13 +6607,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>359</v>
+        <v>336</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
@@ -7231,15 +6626,15 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>571</v>
+        <v>522</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -7251,15 +6646,15 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>361</v>
+        <v>338</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>572</v>
+        <v>523</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -7268,13 +6663,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>362</v>
+        <v>339</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="2"/>
@@ -7287,15 +6682,15 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>573</v>
+        <v>524</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -7307,15 +6702,15 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>574</v>
+        <v>525</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -7327,15 +6722,15 @@
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>575</v>
+        <v>526</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -7344,16 +6739,16 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>366</v>
+        <v>343</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>576</v>
+        <v>527</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -7362,16 +6757,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>577</v>
+        <v>528</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -7380,16 +6775,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>368</v>
+        <v>345</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>578</v>
+        <v>529</v>
       </c>
       <c r="H13" s="2"/>
     </row>
@@ -7398,16 +6793,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>369</v>
+        <v>346</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>579</v>
+        <v>530</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -7419,15 +6814,15 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>370</v>
+        <v>347</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>580</v>
+        <v>531</v>
       </c>
       <c r="H15" s="2"/>
     </row>
@@ -7436,13 +6831,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="2"/>
@@ -7452,7 +6847,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -7468,14 +6863,14 @@
         <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>372</v>
+        <v>349</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>581</v>
+        <v>532</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -7487,14 +6882,14 @@
         <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>582</v>
+        <v>533</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -7506,14 +6901,14 @@
         <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>583</v>
+        <v>534</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -7525,15 +6920,15 @@
         <v>12</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>375</v>
+        <v>352</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>584</v>
+        <v>535</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -7548,11 +6943,11 @@
         <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="2"/>
@@ -7569,13 +6964,13 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>585</v>
+        <v>536</v>
       </c>
       <c r="H23" s="2"/>
     </row>
@@ -7591,13 +6986,13 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>586</v>
+        <v>537</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -7612,11 +7007,11 @@
         <v>12</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
@@ -7635,13 +7030,13 @@
         <v>12</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>587</v>
+        <v>538</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -7659,13 +7054,13 @@
         <v>12</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>588</v>
+        <v>539</v>
       </c>
       <c r="H27" s="2"/>
     </row>
@@ -7677,15 +7072,15 @@
         <v>12</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>589</v>
+        <v>540</v>
       </c>
       <c r="H28" s="2"/>
     </row>
@@ -7697,12 +7092,12 @@
         <v>12</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="2"/>
@@ -7718,14 +7113,14 @@
         <v>12</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>384</v>
+        <v>361</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>590</v>
+        <v>541</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -7740,14 +7135,14 @@
         <v>12</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>591</v>
+        <v>542</v>
       </c>
       <c r="H31" s="2"/>
     </row>
@@ -7759,15 +7154,15 @@
         <v>12</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>592</v>
+        <v>543</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -7783,8 +7178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C748B0E-D4DD-4BAC-8F79-517970D62019}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7795,26 +7190,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
-        <v>458</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>459</v>
+        <v>411</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>412</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="F2" s="17"/>
     </row>
@@ -7827,10 +7222,10 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>593</v>
+        <v>544</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -7843,10 +7238,10 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>594</v>
+        <v>545</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -7859,10 +7254,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>595</v>
+        <v>546</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -7875,10 +7270,10 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>596</v>
+        <v>547</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -7891,7 +7286,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2"/>
@@ -7907,10 +7302,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>597</v>
+        <v>548</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -7925,10 +7320,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>598</v>
+        <v>549</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -7941,10 +7336,10 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>599</v>
+        <v>550</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -7957,10 +7352,10 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>600</v>
+        <v>551</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -7973,10 +7368,10 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>601</v>
+        <v>552</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -7989,10 +7384,10 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>602</v>
+        <v>553</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -8001,10 +7396,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>603</v>
+        <v>554</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -8012,10 +7407,10 @@
         <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>604</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -8030,8 +7425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0491FB6F-EFB8-46A3-A1F8-DBF46D387302}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8040,22 +7435,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -8067,10 +7462,10 @@
         <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>605</v>
+        <v>556</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -8082,10 +7477,10 @@
         <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>606</v>
+        <v>557</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -8097,10 +7492,10 @@
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>607</v>
+        <v>558</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -8112,10 +7507,10 @@
         <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>608</v>
+        <v>559</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -8127,10 +7522,10 @@
         <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>404</v>
+        <v>381</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>609</v>
+        <v>560</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -8142,10 +7537,10 @@
         <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>610</v>
+        <v>561</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -8157,10 +7552,10 @@
         <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>406</v>
+        <v>383</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>611</v>
+        <v>562</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -8172,10 +7567,10 @@
         <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>612</v>
+        <v>563</v>
       </c>
       <c r="E10" s="2"/>
     </row>

</xml_diff>